<commit_message>
hardare section, sensor section
</commit_message>
<xml_diff>
--- a/tables/ProsCons.xlsx
+++ b/tables/ProsCons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-device2\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1744FDD1-D770-4C0C-B0D0-F6CF58E275E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A9F8F5-AC69-4910-8384-E16F4D880158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-19470" windowWidth="29040" windowHeight="15840" xr2:uid="{46186D46-7614-4C3B-A9CF-A71614DFEBF1}"/>
+    <workbookView xWindow="1455" yWindow="30" windowWidth="15120" windowHeight="14790" xr2:uid="{46186D46-7614-4C3B-A9CF-A71614DFEBF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Pros</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>PDF with R-scraping code</t>
+  </si>
+  <si>
+    <t>Exceptional Geo-referencing tools</t>
+  </si>
+  <si>
+    <t>Form building tool requires significant learning time; Trial study could not easilly configure a listing of lengths for review in the field</t>
+  </si>
+  <si>
+    <t>API connectors to external devices requires the Azure license</t>
+  </si>
+  <si>
+    <t>*Connectors to databases including SQL &amp; OneDrive is No-Code (easy to set up) and functions smoothly;   Able to set up on-the-fly editing, listings and frequency plots to review lengths in the field</t>
   </si>
 </sst>
 </file>
@@ -104,8 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,64 +438,76 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>